<commit_message>
Addition of Yahoo Portal Workflows, Excel Workflows
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/359cb36e40a46b53/Documents/UiPath/REF_AutoDesk_Assignment_YahooFinance/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{9ADA8DC4-5857-4028-85F6-AD0B97B8590E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E0744B22-4E96-4FF5-B0E1-8F91965CC2C0}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{9ADA8DC4-5857-4028-85F6-AD0B97B8590E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{89C631F7-F0C3-4E15-A3CF-025EA6B2423E}"/>
   <bookViews>
     <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Name</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>URL for Yahoo Finance</t>
+  </si>
+  <si>
+    <t>ADYF.InputExcelSheetName</t>
+  </si>
+  <si>
+    <t>InputFileSheetName</t>
+  </si>
+  <si>
+    <t>SheetName of Input File</t>
   </si>
 </sst>
 </file>
@@ -2708,7 +2717,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2786,7 +2795,17 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Primary Coding of Process Completed
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/359cb36e40a46b53/Documents/UiPath/REF_AutoDesk_Assignment_YahooFinance/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{9ADA8DC4-5857-4028-85F6-AD0B97B8590E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{89C631F7-F0C3-4E15-A3CF-025EA6B2423E}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{9ADA8DC4-5857-4028-85F6-AD0B97B8590E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FAB8057A-ED9E-430E-9809-E8F181CE7E19}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -154,6 +154,24 @@
   </si>
   <si>
     <t>SheetName of Input File</t>
+  </si>
+  <si>
+    <t>ADYF.OutputReportFolder</t>
+  </si>
+  <si>
+    <t>OutputReportFolder</t>
+  </si>
+  <si>
+    <t>Report Folder where files are downloaded</t>
+  </si>
+  <si>
+    <t>ADYF.OutputExcelFileName</t>
+  </si>
+  <si>
+    <t>ConsolidatedOutputFile</t>
+  </si>
+  <si>
+    <t>File to store the consolidated data from Downloaded reports</t>
   </si>
 </sst>
 </file>
@@ -2717,7 +2735,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2806,8 +2824,28 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Send Email to Business
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/359cb36e40a46b53/Documents/UiPath/REF_AutoDesk_Assignment_YahooFinance/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{9ADA8DC4-5857-4028-85F6-AD0B97B8590E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FAB8057A-ED9E-430E-9809-E8F181CE7E19}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{9ADA8DC4-5857-4028-85F6-AD0B97B8590E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{22A356F9-755A-45B2-9160-59F6CDF9B3FE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -172,6 +172,33 @@
   </si>
   <si>
     <t>File to store the consolidated data from Downloaded reports</t>
+  </si>
+  <si>
+    <t>ADYF.EmailBody</t>
+  </si>
+  <si>
+    <t>EmailBody</t>
+  </si>
+  <si>
+    <t>EmailTo</t>
+  </si>
+  <si>
+    <t>EmailSubject</t>
+  </si>
+  <si>
+    <t>ADYF.EmailTo</t>
+  </si>
+  <si>
+    <t>ADYF.EmailSubject</t>
+  </si>
+  <si>
+    <t>Email Body</t>
+  </si>
+  <si>
+    <t>Email Recepient</t>
+  </si>
+  <si>
+    <t>Email Subject</t>
   </si>
 </sst>
 </file>
@@ -2735,7 +2762,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2846,9 +2873,39 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>